<commit_message>
Renamed the LoginTest bo BankManagerLoginTest
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/excel.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/excel.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Sudhir\GitLocalRepo\DDF\DataDrivenFramework\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -15,8 +20,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>sudhir</t>
+  </si>
+  <si>
+    <t>chakravarthi</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,6 +82,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -105,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -140,7 +168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,12 +377,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>515001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>